<commit_message>
pivot: add reference image to the test files
Change-Id: I2532bae611bc815b270187dc6b9a07b47837962d
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/166383
Tested-by: Tomaž Vajngerl <quikee@gmail.com>
Reviewed-by: Tomaž Vajngerl <quikee@gmail.com>
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/pivot-table/PivotTableCellFormatsTest_10_FormatDefinitionNotMatchingPivotTable.xlsx
+++ b/sc/qa/unit/data/xlsx/pivot-table/PivotTableCellFormatsTest_10_FormatDefinitionNotMatchingPivotTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\quikee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC27F139-E860-480D-B0DA-68EA39449A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D9E3BD-BF00-49FC-8234-3336748238B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="16224" xr2:uid="{D77C3CC8-6808-493C-9198-7EE457FDC5AA}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -81,25 +81,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -118,6 +110,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F73E0160-ABAA-2CB2-E972-C57C6F7A4DE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3048000" y="914400"/>
+          <a:ext cx="1455420" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -275,7 +333,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B5158F5-F24C-4290-B1AB-DF7060F272DC}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B5158F5-F24C-4290-B1AB-DF7060F272DC}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F1:G3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -310,7 +368,7 @@
     <dataField name="Sum of B" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="5">
@@ -636,7 +694,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +724,7 @@
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>60</v>
       </c>
     </row>
@@ -677,7 +735,7 @@
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>60</v>
       </c>
     </row>
@@ -823,5 +881,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>